<commit_message>
Updated the hazards, added some additional assumptions
</commit_message>
<xml_diff>
--- a/org.panorama-research.mobstr.hazards/waters-challenge-2019-hazards.xlsx
+++ b/org.panorama-research.mobstr.hazards/waters-challenge-2019-hazards.xlsx
@@ -1,20 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20371"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20372"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositories\WATERS Challenge Artifacts\org.panorama-research.waters-2019.hazards\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositories\Integrated Safety Analysis\Additional Artifacts\org.panorama-research.mobstr.hazards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFFA7C10-576D-407D-A011-7F313CA895E6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{495A003E-A2E9-496E-A239-A08A69481EDC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Assumptions" sheetId="2" r:id="rId1"/>
-    <sheet name="Hazards" sheetId="1" r:id="rId2"/>
+    <sheet name="Hazards" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="43">
   <si>
     <t>Hazard</t>
   </si>
@@ -107,42 +106,6 @@
   </si>
   <si>
     <t>H-4</t>
-  </si>
-  <si>
-    <t>A-1</t>
-  </si>
-  <si>
-    <t>A-2</t>
-  </si>
-  <si>
-    <t>A-1.1</t>
-  </si>
-  <si>
-    <t>A-3</t>
-  </si>
-  <si>
-    <t>The vehicle has an SAE automation level of 3.</t>
-  </si>
-  <si>
-    <t>The vehicle is used exclusively in urban areas.</t>
-  </si>
-  <si>
-    <t>The vehicle has a normal braking distance of (speed [km/h] / 10)^2.</t>
-  </si>
-  <si>
-    <t>The vehicle has an emergency braking distance of (speed [km/h] / 10)^2 / 2.</t>
-  </si>
-  <si>
-    <t>A-4</t>
-  </si>
-  <si>
-    <t>A-5</t>
-  </si>
-  <si>
-    <t>The vehicle has a minimum (front) sensing range of 100 m.</t>
-  </si>
-  <si>
-    <t>The vehicle drives at a maximum speed of 50 km/h (~ 13.89 m/s).</t>
   </si>
   <si>
     <t>While driving, the vehicle suddenly accelerates without any reason and can collide with an obstacle on or offside the road.</t>
@@ -255,7 +218,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -272,7 +235,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -587,71 +549,6 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="69" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>36</v>
-      </c>
-      <c r="B6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I6"/>
   <sheetViews>
@@ -677,13 +574,13 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>13</v>
@@ -698,21 +595,21 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="7" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" s="6" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>23</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>19</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>5</v>
@@ -727,21 +624,21 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="134.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="123.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>24</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>41</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>53</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>5</v>
@@ -761,16 +658,16 @@
         <v>25</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>4</v>
@@ -785,7 +682,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>26</v>
       </c>
@@ -793,10 +690,10 @@
         <v>17</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>15</v>
@@ -816,13 +713,13 @@
     </row>
     <row r="6" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>21</v>

</xml_diff>